<commit_message>
priority dropdown / khaleel
priority dropdown / khaleel
</commit_message>
<xml_diff>
--- a/03_WeeklyTask/CAL1000 Calyxract Architechture Planning.xlsx
+++ b/03_WeeklyTask/CAL1000 Calyxract Architechture Planning.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t xml:space="preserve">Task no</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve">Objective 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low</t>
   </si>
   <si>
     <t xml:space="preserve">Objective 7</t>
@@ -288,7 +291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -344,12 +347,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -460,19 +457,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -500,10 +489,10 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="E4:E39 B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53"/>
@@ -842,17 +831,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4:E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.65"/>
   </cols>
   <sheetData>
@@ -1005,7 +994,7 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1075,9 +1064,12 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
+      <c r="Q13" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1093,6 +1085,9 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
+      <c r="Q14" s="0" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
@@ -1107,9 +1102,12 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
+      <c r="Q15" s="0" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1125,51 +1123,54 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
+      <c r="Q16" s="0" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1178,16 +1179,16 @@
       <c r="C20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1196,45 +1197,54 @@
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
+      <c r="Q21" s="0" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
+      <c r="Q22" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
+      <c r="Q23" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
-        <v>82</v>
+      <c r="A24" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>38</v>
@@ -1242,17 +1252,17 @@
       <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
-        <v>83</v>
+      <c r="A25" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>41</v>
@@ -1269,7 +1279,7 @@
       <c r="J25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
         <v>43</v>
@@ -1339,8 +1349,8 @@
       <c r="J30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
-        <v>84</v>
+      <c r="A31" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>49</v>
@@ -1371,8 +1381,8 @@
       <c r="J32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="11" t="s">
-        <v>85</v>
+      <c r="A33" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>53</v>
@@ -1475,7 +1485,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="12"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -1487,7 +1497,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="12"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -1499,7 +1509,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="12"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -1511,7 +1521,7 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="12"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -1523,7 +1533,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="12"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -1535,7 +1545,7 @@
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="12"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -1547,7 +1557,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="12"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -1559,7 +1569,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="12"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -1571,7 +1581,7 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="12"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -1582,7 +1592,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
-      <c r="B49" s="15"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -2147,7 +2157,7 @@
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
-      <c r="C96" s="12"/>
+      <c r="C96" s="11"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
@@ -2319,13 +2329,21 @@
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B10:B13"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4:D109" type="list">
-      <formula1>#REF!</formula1>
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D40:D109" type="list">
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4:E109" type="list">
-      <formula1>#REF!</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E40:E109" type="list">
+      <formula1>#ref!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4:D39" type="list">
+      <formula1>'Task and assignment'!$Q$13:$Q$16</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4:E39" type="list">
+      <formula1>'Task and assignment'!$Q$21:$Q$23</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Orientation programming / khaleel
Orientation programming / khaleel
programming as per the flow of flow chart
</commit_message>
<xml_diff>
--- a/03_WeeklyTask/CAL1000 Calyxract Architechture Planning.xlsx
+++ b/03_WeeklyTask/CAL1000 Calyxract Architechture Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Peripheral" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="89">
   <si>
     <t xml:space="preserve">Task no</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">CAN 1-1 interace</t>
   </si>
   <si>
+    <t xml:space="preserve">khaleel</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAN random data send and recieve</t>
   </si>
   <si>
@@ -90,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">GPIO output with stepper motor terminals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">done</t>
   </si>
   <si>
     <t xml:space="preserve">Time to On and Off</t>
@@ -488,11 +494,11 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="E4:E39 B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53"/>
@@ -529,11 +535,17 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -541,274 +553,349 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -833,11 +920,11 @@
   </sheetPr>
   <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4:E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.6"/>
@@ -847,7 +934,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -855,7 +942,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -865,28 +952,28 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +990,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -912,10 +999,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="n">
@@ -929,13 +1016,13 @@
       <c r="A5" s="6"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -949,13 +1036,13 @@
       <c r="A6" s="6"/>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -969,7 +1056,7 @@
       <c r="A7" s="6"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -983,7 +1070,7 @@
       <c r="A8" s="6"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -995,13 +1082,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1015,7 +1102,7 @@
       <c r="A10" s="6"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1028,7 +1115,7 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1041,7 +1128,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1055,7 +1142,7 @@
       <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1065,18 +1152,18 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="Q13" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1086,14 +1173,14 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="Q14" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1103,18 +1190,18 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="Q15" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1124,14 +1211,14 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="Q16" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
@@ -1145,7 +1232,7 @@
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
@@ -1159,7 +1246,7 @@
       <c r="A19" s="11"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
@@ -1171,13 +1258,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1189,13 +1276,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -1205,14 +1292,14 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="Q21" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1222,14 +1309,14 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="Q22" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -1239,18 +1326,18 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="Q23" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -1262,13 +1349,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1282,7 +1369,7 @@
       <c r="A26" s="11"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1296,7 +1383,7 @@
       <c r="A27" s="10"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1310,7 +1397,7 @@
       <c r="A28" s="10"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1324,7 +1411,7 @@
       <c r="A29" s="10"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1338,7 +1425,7 @@
       <c r="A30" s="10"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1350,13 +1437,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1370,7 +1457,7 @@
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1382,13 +1469,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1402,7 +1489,7 @@
       <c r="A34" s="6"/>
       <c r="B34" s="3"/>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1416,7 +1503,7 @@
       <c r="A35" s="10"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1430,7 +1517,7 @@
       <c r="A36" s="6"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1444,7 +1531,7 @@
       <c r="A37" s="6"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1458,7 +1545,7 @@
       <c r="A38" s="6"/>
       <c r="B38" s="3"/>
       <c r="C38" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1472,7 +1559,7 @@
       <c r="A39" s="6"/>
       <c r="B39" s="3"/>
       <c r="C39" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>

</xml_diff>